<commit_message>
new draft sent to NH, AG, SN and OR.
</commit_message>
<xml_diff>
--- a/data/categorization.xlsx
+++ b/data/categorization.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="69">
   <si>
     <t>Heart condition</t>
   </si>
@@ -44,9 +44,6 @@
     <t>Heart infarct</t>
   </si>
   <si>
-    <t>Hypertoni</t>
-  </si>
-  <si>
     <t>hypertension uncomplicated</t>
   </si>
   <si>
@@ -128,9 +125,6 @@
     <t>drug abuse</t>
   </si>
   <si>
-    <t>CNS</t>
-  </si>
-  <si>
     <t>dementia</t>
   </si>
   <si>
@@ -149,9 +143,6 @@
     <t>psychoses</t>
   </si>
   <si>
-    <t>Reuma</t>
-  </si>
-  <si>
     <t>rheumatoid arthritis</t>
   </si>
   <si>
@@ -201,6 +192,45 @@
   </si>
   <si>
     <t>myocardial infarction</t>
+  </si>
+  <si>
+    <t>hypothyroidism</t>
+  </si>
+  <si>
+    <t>coagulopathy</t>
+  </si>
+  <si>
+    <t>obesity</t>
+  </si>
+  <si>
+    <t>weight loss</t>
+  </si>
+  <si>
+    <t>fluid electrolyte disorders</t>
+  </si>
+  <si>
+    <t>Hypothyroidism</t>
+  </si>
+  <si>
+    <t>Coagulopathy</t>
+  </si>
+  <si>
+    <t>Obesity</t>
+  </si>
+  <si>
+    <t>Weight loss</t>
+  </si>
+  <si>
+    <t>Fluid electrolyte disorders</t>
+  </si>
+  <si>
+    <t>Arterial hypertension</t>
+  </si>
+  <si>
+    <t>CNS disease</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rheumatic disease </t>
   </si>
 </sst>
 </file>
@@ -518,28 +548,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C44"/>
+  <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -574,45 +604,45 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B6" t="s">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
         <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
         <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -620,23 +650,23 @@
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -644,23 +674,23 @@
         <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
         <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -668,33 +698,33 @@
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
         <v>18</v>
-      </c>
-      <c r="B18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C18" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -702,23 +732,23 @@
         <v>2</v>
       </c>
       <c r="C21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23" t="s">
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -726,18 +756,18 @@
         <v>2</v>
       </c>
       <c r="C24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" t="s">
         <v>24</v>
-      </c>
-      <c r="B25" t="s">
-        <v>1</v>
-      </c>
-      <c r="C25" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -745,28 +775,28 @@
         <v>2</v>
       </c>
       <c r="C26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" t="s">
         <v>28</v>
-      </c>
-      <c r="B28" t="s">
-        <v>1</v>
-      </c>
-      <c r="C28" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -774,39 +804,39 @@
         <v>2</v>
       </c>
       <c r="C30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>1</v>
+      </c>
+      <c r="C31" t="s">
         <v>31</v>
-      </c>
-      <c r="B31" t="s">
-        <v>1</v>
-      </c>
-      <c r="C31" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>34</v>
+        <v>67</v>
       </c>
       <c r="B33" t="s">
         <v>2</v>
       </c>
       <c r="C33" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -814,33 +844,33 @@
         <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>41</v>
+        <v>68</v>
       </c>
       <c r="B39" t="s">
         <v>1</v>
       </c>
       <c r="C39" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -848,34 +878,34 @@
         <v>2</v>
       </c>
       <c r="C40" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B41" t="s">
         <v>1</v>
       </c>
       <c r="C41" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C42" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B43" t="s">
         <v>1</v>
       </c>
       <c r="C43" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -883,10 +913,66 @@
         <v>2</v>
       </c>
       <c r="C44" t="s">
-        <v>48</v>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>61</v>
+      </c>
+      <c r="B45" t="s">
+        <v>1</v>
+      </c>
+      <c r="C45" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>62</v>
+      </c>
+      <c r="B46" t="s">
+        <v>1</v>
+      </c>
+      <c r="C46" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>63</v>
+      </c>
+      <c r="B47" t="s">
+        <v>1</v>
+      </c>
+      <c r="C47" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>64</v>
+      </c>
+      <c r="B48" t="s">
+        <v>1</v>
+      </c>
+      <c r="C48" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>65</v>
+      </c>
+      <c r="B49" t="s">
+        <v>1</v>
+      </c>
+      <c r="C49" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
version with table 2 combining SHAR and NJR. Updated Shiny app.
</commit_message>
<xml_diff>
--- a/data/categorization.xlsx
+++ b/data/categorization.xlsx
@@ -227,10 +227,10 @@
     <t>Arterial hypertension</t>
   </si>
   <si>
-    <t>CNS disease</t>
-  </si>
-  <si>
     <t xml:space="preserve">Rheumatic disease </t>
+  </si>
+  <si>
+    <t>CNS diseases</t>
   </si>
 </sst>
 </file>
@@ -286,7 +286,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -551,7 +551,7 @@
   <dimension ref="A1:C49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -825,7 +825,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B33" t="s">
         <v>2</v>
@@ -864,7 +864,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B39" t="s">
         <v>1</v>

</xml_diff>